<commit_message>
feat[storage] Add @ExcelFieldName to specify the column name of the resource file
</commit_message>
<xml_diff>
--- a/storage/src/test/resources/excel/StudentResource.xlsx
+++ b/storage/src/test/resources/excel/StudentResource.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17000"/>
+    <workbookView windowWidth="18517" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>age</t>
+    <t>年龄</t>
   </si>
   <si>
     <t>score</t>
@@ -93,12 +93,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,19 +108,49 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -130,16 +160,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -151,40 +174,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -214,45 +206,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,6 +260,114 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -279,175 +380,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,20 +454,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -494,17 +484,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,23 +535,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,148 +554,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -714,54 +707,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1033,14 +1026,14 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" outlineLevelRow="6" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="20.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="109.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.2477876106195" style="1" customWidth="1"/>
+    <col min="6" max="6" width="109.247787610619" style="1" customWidth="1"/>
     <col min="7" max="8" width="49" style="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
[feat] conf json plus
</commit_message>
<xml_diff>
--- a/storage/src/test/resources/excel/StudentResource.xlsx
+++ b/storage/src/test/resources/excel/StudentResource.xlsx
@@ -4,17 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="13515"/>
+    <workbookView windowHeight="23360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>id</t>
   </si>
@@ -43,6 +56,12 @@
     <t>user</t>
   </si>
   <si>
+    <t>arrayValue</t>
+  </si>
+  <si>
+    <t>objectValue</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
@@ -61,6 +80,12 @@
     <t>des</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
     <t>james0</t>
   </si>
   <si>
@@ -74,6 +99,12 @@
   </si>
   <si>
     <t>{"id":"1000","name":"SunInsanity","sex":"boy","age":22}</t>
+  </si>
+  <si>
+    <t>[1,2,4,"5",0.1]</t>
+  </si>
+  <si>
+    <t>{"1":[0],"2":[1],"3":2.0,"4":[]}</t>
   </si>
   <si>
     <t>james1</t>
@@ -106,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -117,7 +148,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -125,7 +156,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -133,14 +164,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -148,7 +179,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -156,7 +187,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -164,7 +195,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -172,7 +203,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -180,14 +211,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -195,7 +226,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -203,7 +234,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -211,14 +242,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -226,42 +257,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -724,55 +755,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1041,23 +1072,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="3" width="9" style="1"/>
     <col min="4" max="4" width="30.2857142857143" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="20.247619047619" style="1" customWidth="1"/>
-    <col min="7" max="7" width="109.247619047619" style="1" customWidth="1"/>
-    <col min="8" max="9" width="49" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="109.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="49" style="1" customWidth="1"/>
+    <col min="9" max="9" width="54.4642857142857" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.9821428571429" customWidth="1"/>
+    <col min="11" max="11" width="39.7321428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,92 +1119,116 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>1000</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1">
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>60.8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1178,28 +1236,28 @@
         <v>1001</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1">
         <v>70.1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1207,28 +1265,28 @@
         <v>1002</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
         <v>80.2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1236,28 +1294,28 @@
         <v>1003</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1">
         <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
perf[storage]: array or collection is null safe
</commit_message>
<xml_diff>
--- a/storage/src/test/resources/excel/StudentResource.xlsx
+++ b/storage/src/test/resources/excel/StudentResource.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>id</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>1, 2, 3</t>
-  </si>
-  <si>
-    <t>[{"id":"1000","name":"SunInsanity","sex":"boy","age":22},{"id":"1000","name":"SunInsanity","sex":"boy","age":25}]</t>
   </si>
   <si>
     <t>james4</t>
@@ -1114,7 +1111,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="K23" sqref="A20:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7"/>
@@ -1127,7 +1124,8 @@
     <col min="8" max="8" width="13.5833333333333" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.25" style="1" customWidth="1"/>
     <col min="10" max="10" width="90.8333333333333" style="1" customWidth="1"/>
-    <col min="11" max="12" width="49" style="1" customWidth="1"/>
+    <col min="11" max="11" width="75.9166666666667" style="1" customWidth="1"/>
+    <col min="12" max="12" width="49" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1358,11 +1356,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>1003</v>
       </c>
-      <c r="B7" s="1"/>
       <c r="C7" s="1">
         <v>13</v>
       </c>
@@ -1381,52 +1378,34 @@
       <c r="H7" s="1">
         <v>1</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>1004</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="1">
         <v>88</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>